<commit_message>
Cambios del generador de redes aleatorias PDF con las notas sobre el material que usamos con las traspas
</commit_message>
<xml_diff>
--- a/slides/materialClases/tema2/generadorRed.xlsx
+++ b/slides/materialClases/tema2/generadorRed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -490,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -522,11 +522,11 @@
       </c>
       <c r="F6" s="1">
         <f ca="1">RAND()</f>
-        <v>0.147364031080088</v>
+        <v>0.60235618081673081</v>
       </c>
       <c r="G6" s="1" t="str">
         <f ca="1">IF(F6&lt;=$C$4,"CON", "NO")</f>
-        <v>CON</v>
+        <v>NO</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -542,11 +542,11 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" ref="F7:F20" ca="1" si="0">RAND()</f>
-        <v>0.3197345838069785</v>
+        <v>0.51907412277904807</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ref="G7:G20" ca="1" si="1">IF(F7&lt;=$C$4,"CON", "NO")</f>
-        <v>CON</v>
+        <v>NO</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -562,11 +562,11 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56664882845363296</v>
+        <v>0.58347333113462363</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CON</v>
+        <v>NO</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88913745506834208</v>
+        <v>0.50836822246507585</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -602,11 +602,11 @@
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14821315789828182</v>
+        <v>0.48538639249146054</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CON</v>
+        <v>NO</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -622,11 +622,11 @@
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36422252410478273</v>
+        <v>0.4008390470392128</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CON</v>
+        <v>NO</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -642,7 +642,7 @@
       </c>
       <c r="F12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86177439978771453</v>
+        <v>0.79258109651628006</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -662,11 +662,11 @@
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.214959860710766</v>
+        <v>0.86331683352343547</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CON</v>
+        <v>NO</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -682,11 +682,11 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21668578390482751</v>
+        <v>0.74260780852405783</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CON</v>
+        <v>NO</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -702,11 +702,11 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49430043000390778</v>
+        <v>0.95555733287667255</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CON</v>
+        <v>NO</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -722,7 +722,7 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32946318120807949</v>
+        <v>6.3509000869318988E-2</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -742,7 +742,7 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.993819957728725</v>
+        <v>0.46446591859817044</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -762,7 +762,7 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96740199021145323</v>
+        <v>0.41867906518447595</v>
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -782,11 +782,11 @@
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21989353894124497</v>
+        <v>0.40983004667515299</v>
       </c>
       <c r="G19" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CON</v>
+        <v>NO</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -802,11 +802,11 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21054899427835083</v>
+        <v>0.66314415438521346</v>
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CON</v>
+        <v>NO</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -821,7 +821,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1">
         <f ca="1">COUNTIF(G6:G20,"CON")</f>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1"/>
     </row>

</xml_diff>